<commit_message>
updated configuration of OpenFAST reference simulations
</commit_message>
<xml_diff>
--- a/sim/openFAST_config_no_inflow.xlsx
+++ b/sim/openFAST_config_no_inflow.xlsx
@@ -59,13 +59,13 @@
     <t xml:space="preserve">Turbsim</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/jgeisler/Temp/ampows/examples/templates/wind/TurbSim.inp</t>
+    <t xml:space="preserve">../5MW_Baseline/wind/TurbSim.inp</t>
   </si>
   <si>
     <t xml:space="preserve">IECWind</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/jgeisler/Temp/ampows/examples/templates/wind/IEC_template.IPT</t>
+    <t xml:space="preserve">../5MW_Baseline/wind/IEC_template.IPT</t>
   </si>
   <si>
     <t xml:space="preserve">Simulation directory</t>
@@ -440,7 +440,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17:B19"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -597,7 +597,7 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="A17:B19 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="B7:B8 A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>